<commit_message>
improving the validator logic + new fix bugs
now there are checks for
- empty strings are replaced with 0 - validation error: 0
- there are characters in the string - validation error
- the upper triangular part of the matrix is not an integer from 1 to 20 (previously from 0 to 5) - validation error
- the lower triangular element is not the inverse of the upper triangular element when multiplied - validation error
- there are no units on the diagonal - validation error

alt_names = alternative_names
</commit_message>
<xml_diff>
--- a/app/algorithms/example/CSV_Tests/Pattern.xlsx
+++ b/app/algorithms/example/CSV_Tests/Pattern.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Programming\Github\6sem\DTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Programming\Github\6sem\DTA\DecisionTheoryApp\app\algorithms\example\CSV_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AA483A2-58EA-4016-A5C3-1AC9181B5AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4856D1-E66D-4046-BC23-DF32695A19A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +718,8 @@
   </sheetPr>
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
       <c r="AA1" s="38"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="AB2" s="8"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
@@ -936,7 +936,7 @@
       </c>
       <c r="AB3" s="16"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="17"/>
       <c r="C4" s="11" t="s">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="AB4" s="16"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="18"/>
       <c r="C5" s="11" t="s">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="AB5" s="16"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AB8" s="16"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="AB9" s="16"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="22" t="s">
         <v>39</v>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="AB10" s="16"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="22" t="s">
         <v>40</v>
@@ -1632,13 +1632,13 @@
       </c>
       <c r="AB11" s="16"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="22" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="23" t="str">
-        <f t="shared" ref="C10:C28" si="11">B12</f>
+        <f t="shared" ref="C12:C28" si="11">B12</f>
         <v>уцйу</v>
       </c>
       <c r="D12" s="21"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB12" s="16"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="22" t="s">
         <v>43</v>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="AB13" s="16"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22" t="s">
         <v>42</v>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="AB14" s="16"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="22" t="s">
         <v>44</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="AB15" s="16"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
         <v>16</v>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="AB16" s="16"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="22" t="s">
         <v>17</v>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="AB17" s="16"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
         <v>19</v>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB18" s="16"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="22" t="s">
         <v>21</v>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="AB19" s="16"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="22" t="s">
         <v>23</v>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="AB20" s="16"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="22" t="s">
         <v>25</v>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="AB21" s="16"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="22" t="s">
         <v>26</v>

</xml_diff>